<commit_message>
Vet change implemented on opioids
</commit_message>
<xml_diff>
--- a/RxNorm/Opioid/Active_Not_Found.xlsx
+++ b/RxNorm/Opioid/Active_Not_Found.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="100">
   <si>
     <t>rxcui</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Imodium Oral Product</t>
   </si>
   <si>
+    <t>Dolorex Solution Injectable Product</t>
+  </si>
+  <si>
     <t>Diamode Oral Product</t>
   </si>
   <si>
@@ -52,6 +55,45 @@
     <t>loperamide hydrochloride 0.133 MG/ML Oral Suspension [Imodium]</t>
   </si>
   <si>
+    <t>butorphanol 10 MG/ML Injectable Solution</t>
+  </si>
+  <si>
+    <t>butorphanol 10 MG/ML Injectable Solution [Dolorex Solution]</t>
+  </si>
+  <si>
+    <t>butorphanol Injectable Solution [Butorphic]</t>
+  </si>
+  <si>
+    <t>Butorphic Injectable Product</t>
+  </si>
+  <si>
+    <t>butorphanol 10 MG/ML Injectable Solution [Butorphic]</t>
+  </si>
+  <si>
+    <t>butorphanol Injectable Solution [Torbugesic]</t>
+  </si>
+  <si>
+    <t>Torbugesic Injectable Product</t>
+  </si>
+  <si>
+    <t>butorphanol 10 MG/ML Injectable Solution [Torbugesic]</t>
+  </si>
+  <si>
+    <t>buprenorphine 1.8 MG/ML Injectable Solution</t>
+  </si>
+  <si>
+    <t>Simbadol Injectable Product</t>
+  </si>
+  <si>
+    <t>buprenorphine 1.8 MG/ML Injectable Solution [Simbadol]</t>
+  </si>
+  <si>
+    <t>butorphanol tartrate 2 MG/ML Injectable Solution [Torbugesic]</t>
+  </si>
+  <si>
+    <t>butorphanol Injectable Solution [Dolorex Solution]</t>
+  </si>
+  <si>
     <t>Kalopanax septemlobus bark extract</t>
   </si>
   <si>
@@ -82,9 +124,6 @@
     <t>belladonna extract, USP / methenamine / salicylamide</t>
   </si>
   <si>
-    <t>belladonna alkaloids / chlorpheniramine / pseudoephedrine</t>
-  </si>
-  <si>
     <t>belladonna alkaloids / caffeine / ergotamine / pentobarbital</t>
   </si>
   <si>
@@ -163,6 +202,9 @@
     <t>SBD</t>
   </si>
   <si>
+    <t>SBDF</t>
+  </si>
+  <si>
     <t>IN</t>
   </si>
   <si>
@@ -181,6 +223,12 @@
     <t>['loperamide']</t>
   </si>
   <si>
+    <t>['butorphanol']</t>
+  </si>
+  <si>
+    <t>['buprenorphine']</t>
+  </si>
+  <si>
     <t>['Kalopanax septemlobus bark extract']</t>
   </si>
   <si>
@@ -206,9 +254,6 @@
   </si>
   <si>
     <t>['methenamine', 'belladonna extract, USP', 'salicylamide']</t>
-  </si>
-  <si>
-    <t>['belladonna alkaloids', 'chlorpheniramine', 'pseudoephedrine']</t>
   </si>
   <si>
     <t>['belladonna alkaloids', 'caffeine', 'ergotamine', 'pentobarbital']</t>
@@ -626,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,13 +702,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -674,13 +719,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -691,13 +736,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -708,625 +753,846 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>1176518</v>
+        <v>1174579</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>1250685</v>
+        <v>1176518</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>1250693</v>
+        <v>1250685</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>1307713</v>
+        <v>1250693</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>6468</v>
+        <v>1302739</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>1006892</v>
+        <v>1302741</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>1007079</v>
+        <v>1310925</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>1007139</v>
+        <v>1310926</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>1007539</v>
+        <v>1310927</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>1007603</v>
+        <v>1489989</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>1007608</v>
+        <v>1489990</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>1007644</v>
+        <v>1489991</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>1007787</v>
+        <v>1594650</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1007825</v>
+        <v>1594654</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>1007893</v>
+        <v>1594655</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>1008045</v>
+        <v>1809204</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>1008287</v>
+        <v>857192</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>1008529</v>
+        <v>1307713</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>1008547</v>
+        <v>6468</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>1008619</v>
+        <v>1006892</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>1008938</v>
+        <v>1007079</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>1009102</v>
+        <v>1007139</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>1043</v>
+        <v>1007539</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>1312380</v>
+        <v>1007603</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>1353220</v>
+        <v>1007608</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>1359</v>
+        <v>1007644</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>1363430</v>
+        <v>1007787</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>1811764</v>
+        <v>1007893</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>215451</v>
+        <v>1008045</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>221074</v>
+        <v>1008287</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>221113</v>
+        <v>1008529</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>314517</v>
+        <v>1008547</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>544581</v>
+        <v>1008619</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <v>71225</v>
+        <v>1008938</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <v>89781</v>
+        <v>1009102</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>42347</v>
+        <v>1043</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
       <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>1312380</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>1353220</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>1359</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>1363430</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>1811764</v>
+      </c>
+      <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="D41" t="s">
+      <c r="C46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>215451</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>221074</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>221113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>314517</v>
+      </c>
+      <c r="B50" t="s">
         <v>53</v>
       </c>
-      <c r="E41" t="s">
-        <v>84</v>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>544581</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>71225</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>89781</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>42347</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>